<commit_message>
updating spring requirements; on wfu
</commit_message>
<xml_diff>
--- a/university_covid_dates.xlsx
+++ b/university_covid_dates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ncris\econ\covid_universities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69AF3BD2-0011-4152-B9C5-3ACF36A6907F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4B4644-EB84-487F-A90F-CD16602ED40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="553">
   <si>
     <t>displayName</t>
   </si>
@@ -1259,27 +1259,15 @@
     <t>https://www.northwestern.edu/coronavirus-covid-19-updates/developments/covid-19-updates-on-vaccination-requirements,-masking-and-testing.html</t>
   </si>
   <si>
-    <t>semester/quarter system?</t>
-  </si>
-  <si>
-    <t>Quarter</t>
-  </si>
-  <si>
     <t>https://www.northwestern.edu/coronavirus-covid-19-updates/developments/updates/spring-break-extended-spring-quarter-remote.html</t>
   </si>
   <si>
-    <t>spring break start date?</t>
-  </si>
-  <si>
     <t>https://covid.dartmouth.edu/march-12-2</t>
   </si>
   <si>
     <t>https://home.dartmouth.edu/news/2021/12/community-message-covid-19-boosters-required-jan-31</t>
   </si>
   <si>
-    <t>sports conference (e.g., ivy league, big ten, etc.)</t>
-  </si>
-  <si>
     <t>https://www.thedartmouth.com/article/2021/04/college-will-require-vaccination-to-return-this-fall</t>
   </si>
   <si>
@@ -1298,9 +1286,6 @@
     <t>Spring 2020 Move Online (first action to move classes online and tell students not to return to campus (some require it); many acted later to extend move to end of semester;)</t>
   </si>
   <si>
-    <t>Date of Spring 2022 Move Online</t>
-  </si>
-  <si>
     <t>Spring 2022 Source</t>
   </si>
   <si>
@@ -1451,9 +1436,6 @@
     <t>https://www.nyu.edu/about/leadership-university-administration/office-of-the-president/office-of-the-provost/provostial-communications/important-news-boosters-required-for-all-nyu-community-members-by-1-18-22.html</t>
   </si>
   <si>
-    <t>Not Yet for Spring, but J-term moved online</t>
-  </si>
-  <si>
     <t>https://www.nyu.edu/about/leadership-university-administration/office-of-the-president/office-of-the-provost/provostial-communications/important-information-summary-update-of-covid-related-developments-at-nyu.html</t>
   </si>
   <si>
@@ -1641,6 +1623,75 @@
   </si>
   <si>
     <t>https://safeandhealthy.osu.edu/messages/2020/03/09/moving-virtual-teaching-and-telework-through-march-30</t>
+  </si>
+  <si>
+    <t>https://covid.princeton.edu/news/2021/change-winter-break-return-dates-undergraduate-students</t>
+  </si>
+  <si>
+    <t>https://covid19.columbia.edu/news/update-start-spring-semester</t>
+  </si>
+  <si>
+    <t>https://www.thecrimson.com/article/2022/1/5/spring-semester-2022-announcement/</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>https://president.yale.edu/president/statements/update-plans-spring-semester</t>
+  </si>
+  <si>
+    <t>https://provost.uchicago.edu/announcements/delayed-start-winter-quarter</t>
+  </si>
+  <si>
+    <t>Date of Spring 2022 Move Online/Delay</t>
+  </si>
+  <si>
+    <t>https://penntoday.upenn.edu/announcements/message-penn-community-regarding-start-spring-semester</t>
+  </si>
+  <si>
+    <t>Ivy</t>
+  </si>
+  <si>
+    <t>https://together.caltech.edu/updates/general/12222021</t>
+  </si>
+  <si>
+    <t>https://coronavirus.duke.edu/2021/12/plans-for-start-of-spring-semester-at-duke/</t>
+  </si>
+  <si>
+    <t>https://www.jhunewsletter.com/article/2022/01/university-updates-covid-19-guidelines-for-spring-2022-semester</t>
+  </si>
+  <si>
+    <t>https://covid.dartmouth.edu/dec29-2021-community-message</t>
+  </si>
+  <si>
+    <t>https://healthy.brown.edu/updates/brown-community-planning-around-covid-19-omicron-variant</t>
+  </si>
+  <si>
+    <t>https://vanderbilthustler.com/44951/featured/breaking-spring-2022-semester-start-date-postponed-testing-protocols-updated/</t>
+  </si>
+  <si>
+    <t>https://statements.cornell.edu/2022/20220106-student-spring-semester.cfm</t>
+  </si>
+  <si>
+    <t>https://news.berkeley.edu/2022/01/07/uc-berkeley-will-begin-spring-semester-with-mostly-remote-instruction/</t>
+  </si>
+  <si>
+    <t>https://record.umich.edu/articles/u-m-will-resume-in-person-classes-jan-5-with-added-safety-measures/</t>
+  </si>
+  <si>
+    <t>https://www.cmu.edu/coronavirus/news-and-communications/communications-archive/2022/january/important-update-about-the-start-of-spring-semester.html</t>
+  </si>
+  <si>
+    <t>https://coronavirus.virginia.edu/updates/important-information-about-spring-start-and-booster-deadline</t>
+  </si>
+  <si>
+    <t>https://www.nyu.edu/about/leadership-university-administration/office-of-the-president/communications/important-timely-taking-stock-update-spring-2022-semester.html</t>
+  </si>
+  <si>
+    <t>https://tuftsdaily.com/news/2022/01/07/breaking-tufts-moves-classes-online-for-first-three-days-of-spring-semester/</t>
+  </si>
+  <si>
+    <t>https://www.unc.edu/posts/2021/12/31/covid-19-update-plans-for-the-spring-2022-semester/</t>
   </si>
 </sst>
 </file>
@@ -2494,28 +2545,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R103"/>
+  <dimension ref="A1:P103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" activeCellId="2" sqref="G1:G1048576 H1:H1048576 I1:I1048576"/>
+    <sheetView tabSelected="1" topLeftCell="G28" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" customWidth="1"/>
-    <col min="6" max="6" width="13.6328125" customWidth="1"/>
-    <col min="7" max="9" width="1.26953125" customWidth="1"/>
-    <col min="10" max="10" width="31" customWidth="1"/>
-    <col min="11" max="11" width="17.81640625" customWidth="1"/>
-    <col min="12" max="12" width="20.90625" customWidth="1"/>
-    <col min="13" max="14" width="15.81640625" customWidth="1"/>
-    <col min="15" max="15" width="15.26953125" customWidth="1"/>
-    <col min="16" max="16" width="28.08984375" customWidth="1"/>
-    <col min="17" max="17" width="15.81640625" customWidth="1"/>
-    <col min="19" max="19" width="8.7265625" customWidth="1"/>
+    <col min="6" max="6" width="8.453125" customWidth="1"/>
+    <col min="7" max="7" width="13.6328125" customWidth="1"/>
+    <col min="8" max="8" width="31" customWidth="1"/>
+    <col min="9" max="9" width="17.81640625" customWidth="1"/>
+    <col min="10" max="10" width="20.90625" customWidth="1"/>
+    <col min="11" max="12" width="15.81640625" customWidth="1"/>
+    <col min="13" max="13" width="15.26953125" customWidth="1"/>
+    <col min="14" max="14" width="28.08984375" customWidth="1"/>
+    <col min="15" max="15" width="15.81640625" customWidth="1"/>
+    <col min="17" max="17" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2532,46 +2583,40 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>538</v>
+      </c>
+      <c r="G1" t="s">
         <v>365</v>
       </c>
-      <c r="G1" t="s">
-        <v>408</v>
-      </c>
       <c r="H1" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="I1" t="s">
+        <v>370</v>
+      </c>
+      <c r="J1" t="s">
         <v>414</v>
       </c>
-      <c r="J1" t="s">
-        <v>420</v>
-      </c>
       <c r="K1" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="L1" t="s">
-        <v>418</v>
+        <v>373</v>
       </c>
       <c r="M1" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="N1" t="s">
-        <v>373</v>
+        <v>536</v>
       </c>
       <c r="O1" t="s">
-        <v>374</v>
+        <v>417</v>
       </c>
       <c r="P1" t="s">
-        <v>421</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>422</v>
-      </c>
-      <c r="R1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2587,34 +2632,41 @@
       <c r="E2">
         <v>8544</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>366</v>
       </c>
-      <c r="J2" s="2">
+      <c r="H2" s="2">
         <v>43901</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="J2" s="3">
+        <v>44306</v>
+      </c>
       <c r="K2" s="1" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="L2" s="3">
-        <v>44306</v>
+        <v>44546</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="N2" s="3">
-        <v>44546</v>
+        <v>44557</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" t="s">
+        <v>530</v>
+      </c>
+      <c r="P2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -2630,32 +2682,41 @@
       <c r="E3">
         <v>10027</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>366</v>
       </c>
+      <c r="H3" s="2">
+        <v>43902</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>378</v>
+      </c>
       <c r="J3" s="2">
-        <v>43902</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>378</v>
+        <v>44305</v>
+      </c>
+      <c r="K3" t="s">
+        <v>377</v>
       </c>
       <c r="L3" s="2">
-        <v>44305</v>
+        <v>44546</v>
       </c>
       <c r="M3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="N3" s="2">
-        <v>44546</v>
+        <v>44552</v>
       </c>
       <c r="O3" t="s">
-        <v>376</v>
-      </c>
-      <c r="R3" t="s">
+        <v>531</v>
+      </c>
+      <c r="P3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2671,32 +2732,41 @@
       <c r="E4">
         <v>2138</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
         <v>366</v>
       </c>
+      <c r="H4" s="2">
+        <v>43900</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>381</v>
+      </c>
       <c r="J4" s="2">
-        <v>43900</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>381</v>
+        <v>44321</v>
+      </c>
+      <c r="K4" t="s">
+        <v>380</v>
       </c>
       <c r="L4" s="2">
-        <v>44321</v>
+        <v>44546</v>
       </c>
       <c r="M4" t="s">
-        <v>380</v>
-      </c>
-      <c r="N4" s="2">
-        <v>44546</v>
+        <v>379</v>
+      </c>
+      <c r="N4" t="s">
+        <v>533</v>
       </c>
       <c r="O4" t="s">
-        <v>379</v>
-      </c>
-      <c r="R4" t="s">
+        <v>532</v>
+      </c>
+      <c r="P4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2712,32 +2782,38 @@
       <c r="E5">
         <v>2139</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
         <v>366</v>
       </c>
+      <c r="H5" s="2">
+        <v>43900</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>384</v>
+      </c>
       <c r="J5" s="2">
-        <v>43900</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>384</v>
+        <v>44316</v>
+      </c>
+      <c r="K5" t="s">
+        <v>383</v>
       </c>
       <c r="L5" s="2">
-        <v>44316</v>
+        <v>44543</v>
       </c>
       <c r="M5" t="s">
-        <v>383</v>
-      </c>
-      <c r="N5" s="2">
-        <v>44543</v>
-      </c>
-      <c r="O5" t="s">
         <v>382</v>
       </c>
-      <c r="R5" t="s">
+      <c r="N5" t="s">
+        <v>533</v>
+      </c>
+      <c r="P5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -2753,34 +2829,41 @@
       <c r="E6">
         <v>6520</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
         <v>366</v>
       </c>
+      <c r="H6" s="2">
+        <v>43900</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="J6" s="2">
-        <v>43900</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>385</v>
+        <v>44305</v>
+      </c>
+      <c r="K6" t="s">
+        <v>386</v>
       </c>
       <c r="L6" s="2">
-        <v>44305</v>
-      </c>
-      <c r="M6" t="s">
-        <v>386</v>
-      </c>
-      <c r="N6" s="2">
         <v>44547</v>
       </c>
+      <c r="M6" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="N6" s="3">
+        <v>44552</v>
+      </c>
       <c r="O6" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" t="s">
+        <v>534</v>
+      </c>
+      <c r="P6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -2796,34 +2879,41 @@
       <c r="E7">
         <v>94305</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
         <v>366</v>
       </c>
+      <c r="H7" s="2">
+        <v>43903</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>390</v>
+      </c>
       <c r="J7" s="2">
-        <v>43903</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>390</v>
+        <v>44308</v>
+      </c>
+      <c r="K7" t="s">
+        <v>389</v>
       </c>
       <c r="L7" s="2">
-        <v>44308</v>
-      </c>
-      <c r="M7" t="s">
-        <v>389</v>
-      </c>
-      <c r="N7" s="2">
+        <v>44546</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="N7" s="3">
         <v>44546</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" t="s">
+      <c r="P7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -2839,32 +2929,41 @@
       <c r="E8">
         <v>60637</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
         <v>366</v>
       </c>
+      <c r="H8" s="2">
+        <v>43902</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>391</v>
+      </c>
       <c r="J8" s="2">
-        <v>43902</v>
+        <v>44334</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="L8" s="2">
-        <v>44334</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>392</v>
+        <v>44550</v>
+      </c>
+      <c r="M8" t="s">
+        <v>393</v>
       </c>
       <c r="N8" s="2">
-        <v>44550</v>
+        <v>44553</v>
       </c>
       <c r="O8" t="s">
-        <v>393</v>
-      </c>
-      <c r="R8" t="s">
+        <v>535</v>
+      </c>
+      <c r="P8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -2880,32 +2979,41 @@
       <c r="E9">
         <v>19104</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
         <v>366</v>
       </c>
+      <c r="H9" s="2">
+        <v>43901</v>
+      </c>
+      <c r="I9" t="s">
+        <v>396</v>
+      </c>
       <c r="J9" s="2">
-        <v>43901</v>
+        <v>44308</v>
       </c>
       <c r="K9" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L9" s="2">
-        <v>44308</v>
+        <v>44551</v>
       </c>
       <c r="M9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="N9" s="2">
-        <v>44551</v>
+        <v>44553</v>
       </c>
       <c r="O9" t="s">
-        <v>394</v>
-      </c>
-      <c r="R9" t="s">
+        <v>537</v>
+      </c>
+      <c r="P9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -2921,32 +3029,41 @@
       <c r="E10">
         <v>91125</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
         <v>366</v>
       </c>
+      <c r="H10" s="2">
+        <v>43903</v>
+      </c>
+      <c r="I10" t="s">
+        <v>399</v>
+      </c>
       <c r="J10" s="2">
-        <v>43903</v>
+        <v>44312</v>
       </c>
       <c r="K10" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="L10" s="2">
-        <v>44312</v>
+        <v>44547</v>
       </c>
       <c r="M10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="N10" s="2">
-        <v>44547</v>
+        <v>44552</v>
       </c>
       <c r="O10" t="s">
-        <v>397</v>
-      </c>
-      <c r="R10" t="s">
+        <v>539</v>
+      </c>
+      <c r="P10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -2962,32 +3079,41 @@
       <c r="E11">
         <v>27708</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
         <v>366</v>
       </c>
+      <c r="H11" s="2">
+        <v>43900</v>
+      </c>
+      <c r="I11" t="s">
+        <v>402</v>
+      </c>
       <c r="J11" s="2">
-        <v>43900</v>
+        <v>44295</v>
       </c>
       <c r="K11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="L11" s="2">
-        <v>44295</v>
+        <v>44550</v>
       </c>
       <c r="M11" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="N11" s="2">
-        <v>44550</v>
+        <v>44552</v>
       </c>
       <c r="O11" t="s">
-        <v>400</v>
-      </c>
-      <c r="R11" t="s">
+        <v>540</v>
+      </c>
+      <c r="P11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -3003,32 +3129,41 @@
       <c r="E12">
         <v>21218</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
         <v>366</v>
       </c>
+      <c r="H12" s="2">
+        <v>43900</v>
+      </c>
+      <c r="I12" t="s">
+        <v>405</v>
+      </c>
       <c r="J12" s="2">
-        <v>43900</v>
+        <v>44295</v>
       </c>
       <c r="K12" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L12" s="2">
-        <v>44295</v>
+        <v>44551</v>
       </c>
       <c r="M12" t="s">
-        <v>404</v>
-      </c>
-      <c r="N12" s="2">
-        <v>44551</v>
+        <v>403</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>533</v>
       </c>
       <c r="O12" t="s">
-        <v>403</v>
-      </c>
-      <c r="R12" t="s">
+        <v>541</v>
+      </c>
+      <c r="P12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>53</v>
       </c>
@@ -3044,23 +3179,29 @@
       <c r="E13">
         <v>60208</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
         <v>366</v>
       </c>
-      <c r="G13" t="s">
-        <v>409</v>
+      <c r="H13" s="2">
+        <v>43901</v>
+      </c>
+      <c r="I13" t="s">
+        <v>408</v>
       </c>
       <c r="J13" s="2">
-        <v>43901</v>
+        <v>44328</v>
       </c>
       <c r="K13" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="L13" s="2">
-        <v>44328</v>
+        <v>44550</v>
       </c>
       <c r="M13" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="N13" s="2">
         <v>44550</v>
@@ -3068,11 +3209,11 @@
       <c r="O13" t="s">
         <v>406</v>
       </c>
-      <c r="R13" t="s">
+      <c r="P13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -3088,32 +3229,41 @@
       <c r="E14">
         <v>3755</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
         <v>366</v>
       </c>
+      <c r="H14" s="2">
+        <v>43902</v>
+      </c>
+      <c r="I14" t="s">
+        <v>409</v>
+      </c>
       <c r="J14" s="2">
-        <v>43902</v>
+        <v>44300</v>
       </c>
       <c r="K14" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="L14" s="2">
-        <v>44300</v>
+        <v>44547</v>
       </c>
       <c r="M14" t="s">
-        <v>415</v>
-      </c>
-      <c r="N14" s="2">
-        <v>44547</v>
+        <v>410</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>533</v>
       </c>
       <c r="O14" t="s">
-        <v>413</v>
-      </c>
-      <c r="R14" t="s">
+        <v>542</v>
+      </c>
+      <c r="P14" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>61</v>
       </c>
@@ -3129,32 +3279,41 @@
       <c r="E15">
         <v>2912</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
         <v>366</v>
       </c>
+      <c r="H15" s="2">
+        <v>43902</v>
+      </c>
+      <c r="I15" t="s">
+        <v>415</v>
+      </c>
       <c r="J15" s="2">
-        <v>43902</v>
+        <v>44292</v>
       </c>
       <c r="K15" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="L15" s="2">
-        <v>44292</v>
+        <v>44544</v>
       </c>
       <c r="M15" t="s">
-        <v>417</v>
-      </c>
-      <c r="N15" s="2">
-        <v>44544</v>
+        <v>412</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>533</v>
       </c>
       <c r="O15" t="s">
-        <v>416</v>
-      </c>
-      <c r="R15" t="s">
+        <v>543</v>
+      </c>
+      <c r="P15" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>66</v>
       </c>
@@ -3170,32 +3329,38 @@
       <c r="E16">
         <v>37240</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
         <v>366</v>
       </c>
+      <c r="H16" s="2">
+        <v>43899</v>
+      </c>
+      <c r="I16" t="s">
+        <v>420</v>
+      </c>
       <c r="J16" s="2">
-        <v>43899</v>
+        <v>44333</v>
       </c>
       <c r="K16" t="s">
-        <v>425</v>
-      </c>
-      <c r="L16" s="2">
-        <v>44333</v>
-      </c>
-      <c r="M16" t="s">
-        <v>424</v>
-      </c>
-      <c r="N16" t="s">
-        <v>423</v>
+        <v>419</v>
+      </c>
+      <c r="L16" t="s">
+        <v>418</v>
+      </c>
+      <c r="N16" s="2">
+        <v>44560</v>
+      </c>
+      <c r="O16" t="s">
+        <v>544</v>
       </c>
       <c r="P16" t="s">
-        <v>423</v>
-      </c>
-      <c r="R16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>70</v>
       </c>
@@ -3211,35 +3376,38 @@
       <c r="E17">
         <v>63130</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
         <v>366</v>
       </c>
+      <c r="H17" s="2">
+        <v>43901</v>
+      </c>
+      <c r="I17" t="s">
+        <v>423</v>
+      </c>
       <c r="J17" s="2">
-        <v>43901</v>
-      </c>
-      <c r="K17" t="s">
-        <v>428</v>
-      </c>
-      <c r="L17" s="2">
         <v>44314</v>
       </c>
-      <c r="M17" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="N17" t="s">
-        <v>423</v>
-      </c>
-      <c r="P17" s="2">
+      <c r="K17" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="L17" t="s">
+        <v>418</v>
+      </c>
+      <c r="N17" s="2">
         <v>44560</v>
       </c>
-      <c r="Q17" t="s">
-        <v>426</v>
-      </c>
-      <c r="R17" t="s">
+      <c r="O17" t="s">
+        <v>421</v>
+      </c>
+      <c r="P17" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>74</v>
       </c>
@@ -3255,35 +3423,41 @@
       <c r="E18">
         <v>14853</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
         <v>366</v>
       </c>
+      <c r="H18" s="2">
+        <v>43903</v>
+      </c>
+      <c r="I18" t="s">
+        <v>426</v>
+      </c>
       <c r="J18" s="2">
-        <v>43903</v>
+        <v>44288</v>
       </c>
       <c r="K18" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="L18" s="2">
-        <v>44288</v>
+        <v>44551</v>
       </c>
       <c r="M18" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="N18" s="2">
-        <v>44551</v>
+        <v>44567</v>
       </c>
       <c r="O18" t="s">
-        <v>429</v>
+        <v>545</v>
       </c>
       <c r="P18" t="s">
-        <v>423</v>
-      </c>
-      <c r="R18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -3299,38 +3473,41 @@
       <c r="E19">
         <v>77251</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
         <v>366</v>
       </c>
+      <c r="H19" s="2">
+        <v>43902</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>428</v>
+      </c>
       <c r="J19" s="2">
-        <v>43902</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>433</v>
+        <v>44344</v>
+      </c>
+      <c r="K19" t="s">
+        <v>429</v>
       </c>
       <c r="L19" s="2">
-        <v>44344</v>
+        <v>44556</v>
       </c>
       <c r="M19" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="N19" s="2">
         <v>44556</v>
       </c>
       <c r="O19" t="s">
-        <v>432</v>
-      </c>
-      <c r="P19" s="2">
-        <v>44556</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>432</v>
-      </c>
-      <c r="R19" t="s">
+        <v>427</v>
+      </c>
+      <c r="P19" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -3346,32 +3523,38 @@
       <c r="E20">
         <v>46556</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
         <v>366</v>
       </c>
+      <c r="H20" s="2">
+        <v>43901</v>
+      </c>
+      <c r="I20" t="s">
+        <v>432</v>
+      </c>
       <c r="J20" s="2">
-        <v>43901</v>
+        <v>44293</v>
       </c>
       <c r="K20" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="L20" s="2">
-        <v>44293</v>
+        <v>44536</v>
       </c>
       <c r="M20" t="s">
-        <v>436</v>
-      </c>
-      <c r="N20" s="2">
-        <v>44536</v>
-      </c>
-      <c r="O20" t="s">
-        <v>435</v>
-      </c>
-      <c r="R20" t="s">
+        <v>430</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="P20" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>87</v>
       </c>
@@ -3387,38 +3570,41 @@
       <c r="E21">
         <v>90095</v>
       </c>
-      <c r="F21" t="s">
-        <v>457</v>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>452</v>
+      </c>
+      <c r="H21" s="2">
+        <v>43900</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>434</v>
       </c>
       <c r="J21" s="2">
-        <v>43900</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>439</v>
+        <v>44392</v>
+      </c>
+      <c r="K21" t="s">
+        <v>433</v>
       </c>
       <c r="L21" s="2">
-        <v>44392</v>
+        <v>44551</v>
       </c>
       <c r="M21" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="N21" s="2">
         <v>44551</v>
       </c>
       <c r="O21" t="s">
-        <v>440</v>
-      </c>
-      <c r="P21" s="2">
-        <v>44551</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>440</v>
-      </c>
-      <c r="R21" t="s">
+        <v>435</v>
+      </c>
+      <c r="P21" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>91</v>
       </c>
@@ -3434,38 +3620,41 @@
       <c r="E22">
         <v>30322</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
         <v>366</v>
       </c>
+      <c r="H22" s="2">
+        <v>43901</v>
+      </c>
+      <c r="I22" t="s">
+        <v>440</v>
+      </c>
       <c r="J22" s="2">
-        <v>43901</v>
+        <v>44305</v>
       </c>
       <c r="K22" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="L22" s="2">
-        <v>44305</v>
+        <v>44546</v>
       </c>
       <c r="M22" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="N22" s="2">
-        <v>44546</v>
+        <v>44558</v>
       </c>
       <c r="O22" t="s">
-        <v>442</v>
-      </c>
-      <c r="P22" s="2">
-        <v>44558</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>443</v>
-      </c>
-      <c r="R22" t="s">
+        <v>438</v>
+      </c>
+      <c r="P22" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>96</v>
       </c>
@@ -3481,35 +3670,41 @@
       <c r="E23">
         <v>94720</v>
       </c>
-      <c r="F23" t="s">
-        <v>457</v>
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>452</v>
+      </c>
+      <c r="H23" s="2">
+        <v>43899</v>
+      </c>
+      <c r="I23" t="s">
+        <v>442</v>
       </c>
       <c r="J23" s="2">
-        <v>43899</v>
-      </c>
-      <c r="K23" t="s">
-        <v>447</v>
+        <v>44392</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>433</v>
       </c>
       <c r="L23" s="2">
-        <v>44392</v>
+        <v>44551</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="N23" s="2">
-        <v>44551</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>446</v>
+        <v>44568</v>
+      </c>
+      <c r="O23" t="s">
+        <v>546</v>
       </c>
       <c r="P23" t="s">
-        <v>423</v>
-      </c>
-      <c r="R23" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>100</v>
       </c>
@@ -3525,38 +3720,41 @@
       <c r="E24">
         <v>20057</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" t="s">
         <v>366</v>
       </c>
+      <c r="H24" s="2">
+        <v>43901</v>
+      </c>
+      <c r="I24" t="s">
+        <v>447</v>
+      </c>
       <c r="J24" s="2">
-        <v>43901</v>
+        <v>44300</v>
       </c>
       <c r="K24" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
       <c r="L24" s="2">
-        <v>44300</v>
+        <v>44544</v>
       </c>
       <c r="M24" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
       <c r="N24" s="2">
-        <v>44544</v>
+        <v>44559</v>
       </c>
       <c r="O24" t="s">
-        <v>450</v>
-      </c>
-      <c r="P24" s="2">
-        <v>44559</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>449</v>
-      </c>
-      <c r="R24" t="s">
+        <v>444</v>
+      </c>
+      <c r="P24" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>105</v>
       </c>
@@ -3572,35 +3770,41 @@
       <c r="E25">
         <v>48109</v>
       </c>
-      <c r="F25" t="s">
-        <v>457</v>
+      <c r="F25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" t="s">
+        <v>452</v>
+      </c>
+      <c r="H25" s="2">
+        <v>43901</v>
+      </c>
+      <c r="I25" t="s">
+        <v>449</v>
       </c>
       <c r="J25" s="2">
-        <v>43901</v>
+        <v>44407</v>
       </c>
       <c r="K25" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="L25" s="2">
-        <v>44407</v>
+        <v>44547</v>
       </c>
       <c r="M25" t="s">
-        <v>456</v>
-      </c>
-      <c r="N25" s="2">
-        <v>44547</v>
+        <v>448</v>
+      </c>
+      <c r="N25" t="s">
+        <v>533</v>
       </c>
       <c r="O25" t="s">
-        <v>453</v>
+        <v>547</v>
       </c>
       <c r="P25" t="s">
-        <v>423</v>
-      </c>
-      <c r="R25" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>109</v>
       </c>
@@ -3616,35 +3820,41 @@
       <c r="E26">
         <v>15213</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" t="b">
+        <v>0</v>
+      </c>
+      <c r="G26" t="s">
         <v>366</v>
       </c>
+      <c r="H26" s="2">
+        <v>43901</v>
+      </c>
+      <c r="I26" t="s">
+        <v>455</v>
+      </c>
       <c r="J26" s="2">
-        <v>43901</v>
+        <v>44327</v>
       </c>
       <c r="K26" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="L26" s="2">
-        <v>44327</v>
+        <v>44546</v>
       </c>
       <c r="M26" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="N26" s="2">
-        <v>44546</v>
+        <v>44567</v>
       </c>
       <c r="O26" t="s">
-        <v>458</v>
-      </c>
-      <c r="P26" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="R26" t="s">
+        <v>548</v>
+      </c>
+      <c r="P26" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>113</v>
       </c>
@@ -3660,35 +3870,41 @@
       <c r="E27">
         <v>22904</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" t="s">
+        <v>452</v>
+      </c>
+      <c r="H27" s="2">
+        <v>43901</v>
+      </c>
+      <c r="I27" t="s">
+        <v>458</v>
+      </c>
+      <c r="J27" s="2">
+        <v>44336</v>
+      </c>
+      <c r="K27" t="s">
         <v>457</v>
       </c>
-      <c r="J27" s="2">
-        <v>43901</v>
-      </c>
-      <c r="K27" t="s">
-        <v>463</v>
-      </c>
       <c r="L27" s="2">
-        <v>44336</v>
+        <v>44551</v>
       </c>
       <c r="M27" t="s">
-        <v>462</v>
-      </c>
-      <c r="N27" s="2">
-        <v>44551</v>
+        <v>456</v>
+      </c>
+      <c r="N27" t="s">
+        <v>533</v>
       </c>
       <c r="O27" t="s">
-        <v>461</v>
+        <v>549</v>
       </c>
       <c r="P27" t="s">
-        <v>423</v>
-      </c>
-      <c r="R27" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>117</v>
       </c>
@@ -3704,38 +3920,41 @@
       <c r="E28">
         <v>90089</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" t="b">
+        <v>0</v>
+      </c>
+      <c r="G28" t="s">
         <v>366</v>
       </c>
+      <c r="H28" s="2">
+        <v>43896</v>
+      </c>
+      <c r="I28" t="s">
+        <v>461</v>
+      </c>
       <c r="J28" s="2">
-        <v>43896</v>
+        <v>44364</v>
       </c>
       <c r="K28" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="L28" s="2">
-        <v>44364</v>
+        <v>44558</v>
       </c>
       <c r="M28" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
       <c r="N28" s="2">
-        <v>44558</v>
+        <v>44554</v>
       </c>
       <c r="O28" t="s">
-        <v>464</v>
-      </c>
-      <c r="P28" s="2">
-        <v>44554</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>465</v>
-      </c>
-      <c r="R28" t="s">
+        <v>460</v>
+      </c>
+      <c r="P28" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>120</v>
       </c>
@@ -3751,35 +3970,41 @@
       <c r="E29">
         <v>10012</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" t="b">
+        <v>0</v>
+      </c>
+      <c r="G29" t="s">
         <v>366</v>
       </c>
+      <c r="H29" s="2">
+        <v>43899</v>
+      </c>
+      <c r="I29" t="s">
+        <v>468</v>
+      </c>
       <c r="J29" s="2">
-        <v>43899</v>
+        <v>44305</v>
       </c>
       <c r="K29" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="L29" s="2">
-        <v>44305</v>
+        <v>44544</v>
       </c>
       <c r="M29" t="s">
-        <v>473</v>
-      </c>
-      <c r="N29" s="2">
-        <v>44544</v>
+        <v>466</v>
+      </c>
+      <c r="N29" t="s">
+        <v>533</v>
       </c>
       <c r="O29" t="s">
-        <v>471</v>
+        <v>550</v>
       </c>
       <c r="P29" t="s">
-        <v>472</v>
-      </c>
-      <c r="R29" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>123</v>
       </c>
@@ -3795,35 +4020,41 @@
       <c r="E30">
         <v>2155</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" t="b">
+        <v>0</v>
+      </c>
+      <c r="G30" t="s">
         <v>366</v>
       </c>
+      <c r="H30" s="2">
+        <v>43900</v>
+      </c>
+      <c r="I30" t="s">
+        <v>471</v>
+      </c>
       <c r="J30" s="2">
-        <v>43900</v>
+        <v>44311</v>
       </c>
       <c r="K30" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="L30" s="2">
-        <v>44311</v>
+        <v>44547</v>
       </c>
       <c r="M30" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="N30" s="2">
-        <v>44547</v>
+        <v>44568</v>
       </c>
       <c r="O30" t="s">
-        <v>475</v>
-      </c>
-      <c r="P30" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="R30" t="s">
+        <v>551</v>
+      </c>
+      <c r="P30" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>126</v>
       </c>
@@ -3839,38 +4070,41 @@
       <c r="E31">
         <v>93106</v>
       </c>
-      <c r="F31" t="s">
-        <v>457</v>
+      <c r="F31" t="b">
+        <v>0</v>
+      </c>
+      <c r="G31" t="s">
+        <v>452</v>
+      </c>
+      <c r="H31" s="2">
+        <v>43900</v>
+      </c>
+      <c r="I31" t="s">
+        <v>474</v>
       </c>
       <c r="J31" s="2">
-        <v>43900</v>
+        <v>44392</v>
       </c>
       <c r="K31" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
       <c r="L31" s="2">
-        <v>44392</v>
+        <v>44551</v>
       </c>
       <c r="M31" t="s">
-        <v>479</v>
+        <v>441</v>
       </c>
       <c r="N31" s="2">
         <v>44551</v>
       </c>
       <c r="O31" t="s">
-        <v>446</v>
-      </c>
-      <c r="P31" s="2">
-        <v>44551</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>478</v>
-      </c>
-      <c r="R31" t="s">
+        <v>472</v>
+      </c>
+      <c r="P31" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>129</v>
       </c>
@@ -3886,29 +4120,32 @@
       <c r="E32">
         <v>32611</v>
       </c>
-      <c r="F32" t="s">
-        <v>457</v>
-      </c>
-      <c r="J32" s="2">
+      <c r="F32" t="b">
+        <v>0</v>
+      </c>
+      <c r="G32" t="s">
+        <v>452</v>
+      </c>
+      <c r="H32" s="2">
         <v>43901</v>
       </c>
-      <c r="K32" t="s">
-        <v>481</v>
+      <c r="I32" t="s">
+        <v>475</v>
+      </c>
+      <c r="J32" t="s">
+        <v>418</v>
       </c>
       <c r="L32" t="s">
-        <v>423</v>
-      </c>
-      <c r="N32" t="s">
-        <v>423</v>
-      </c>
-      <c r="P32" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="R32" t="s">
+        <v>418</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="P32" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>133</v>
       </c>
@@ -3924,29 +4161,35 @@
       <c r="E33">
         <v>27599</v>
       </c>
-      <c r="F33" t="s">
-        <v>457</v>
-      </c>
-      <c r="J33" s="2">
+      <c r="F33" t="b">
+        <v>0</v>
+      </c>
+      <c r="G33" t="s">
+        <v>452</v>
+      </c>
+      <c r="H33" s="2">
         <v>43901</v>
       </c>
-      <c r="K33" t="s">
-        <v>482</v>
+      <c r="I33" t="s">
+        <v>476</v>
+      </c>
+      <c r="J33" t="s">
+        <v>418</v>
       </c>
       <c r="L33" t="s">
-        <v>423</v>
-      </c>
-      <c r="N33" t="s">
-        <v>423</v>
-      </c>
-      <c r="P33" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="R33" t="s">
+        <v>418</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="O33" t="s">
+        <v>552</v>
+      </c>
+      <c r="P33" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>136</v>
       </c>
@@ -3962,35 +4205,38 @@
       <c r="E34">
         <v>27109</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" t="b">
+        <v>0</v>
+      </c>
+      <c r="G34" t="s">
         <v>366</v>
       </c>
+      <c r="H34" s="2">
+        <v>43901</v>
+      </c>
+      <c r="I34" t="s">
+        <v>479</v>
+      </c>
       <c r="J34" s="2">
-        <v>43901</v>
+        <v>44306</v>
       </c>
       <c r="K34" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="L34" s="2">
-        <v>44306</v>
+        <v>44540</v>
       </c>
       <c r="M34" t="s">
-        <v>484</v>
-      </c>
-      <c r="N34" s="2">
-        <v>44540</v>
-      </c>
-      <c r="O34" t="s">
-        <v>483</v>
-      </c>
-      <c r="P34" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="R34" t="s">
+        <v>477</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="P34" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>139</v>
       </c>
@@ -4006,35 +4252,38 @@
       <c r="E35">
         <v>92093</v>
       </c>
-      <c r="F35" t="s">
-        <v>457</v>
+      <c r="F35" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" t="s">
+        <v>452</v>
+      </c>
+      <c r="H35" s="2">
+        <v>43899</v>
+      </c>
+      <c r="I35" t="s">
+        <v>481</v>
       </c>
       <c r="J35" s="2">
-        <v>43899</v>
+        <v>44392</v>
       </c>
       <c r="K35" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
       <c r="L35" s="2">
-        <v>44392</v>
+        <v>44551</v>
       </c>
       <c r="M35" t="s">
-        <v>486</v>
-      </c>
-      <c r="N35" s="2">
-        <v>44551</v>
-      </c>
-      <c r="O35" t="s">
-        <v>446</v>
-      </c>
-      <c r="P35" s="2" t="s">
-        <v>488</v>
-      </c>
-      <c r="R35" t="s">
+        <v>441</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="P35" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>143</v>
       </c>
@@ -4050,35 +4299,38 @@
       <c r="E36">
         <v>14627</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" t="b">
+        <v>0</v>
+      </c>
+      <c r="G36" t="s">
         <v>366</v>
       </c>
+      <c r="H36" s="2">
+        <v>43901</v>
+      </c>
+      <c r="I36" t="s">
+        <v>485</v>
+      </c>
       <c r="J36" s="2">
-        <v>43901</v>
+        <v>44308</v>
       </c>
       <c r="K36" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="L36" s="2">
-        <v>44308</v>
+        <v>44553</v>
       </c>
       <c r="M36" t="s">
-        <v>490</v>
-      </c>
-      <c r="N36" s="2">
-        <v>44553</v>
-      </c>
-      <c r="O36" t="s">
-        <v>489</v>
-      </c>
-      <c r="P36" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="R36" t="s">
+        <v>483</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="P36" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>146</v>
       </c>
@@ -4094,32 +4346,35 @@
       <c r="E37">
         <v>2467</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" t="b">
+        <v>0</v>
+      </c>
+      <c r="G37" t="s">
         <v>366</v>
       </c>
+      <c r="H37" s="2">
+        <v>43901</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="J37" s="2">
-        <v>43901</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>494</v>
+        <v>44309</v>
+      </c>
+      <c r="K37" t="s">
+        <v>487</v>
       </c>
       <c r="L37" s="2">
-        <v>44309</v>
+        <v>44544</v>
       </c>
       <c r="M37" t="s">
-        <v>493</v>
-      </c>
-      <c r="N37" s="2">
-        <v>44544</v>
-      </c>
-      <c r="O37" t="s">
-        <v>492</v>
-      </c>
-      <c r="R37" t="s">
+        <v>486</v>
+      </c>
+      <c r="P37" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -4135,38 +4390,41 @@
       <c r="E38">
         <v>92697</v>
       </c>
-      <c r="F38" t="s">
-        <v>457</v>
+      <c r="F38" t="b">
+        <v>0</v>
+      </c>
+      <c r="G38" t="s">
+        <v>452</v>
+      </c>
+      <c r="H38" s="2">
+        <v>43900</v>
+      </c>
+      <c r="I38" t="s">
+        <v>490</v>
       </c>
       <c r="J38" s="2">
-        <v>43900</v>
+        <v>44392</v>
       </c>
       <c r="K38" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="L38" s="2">
-        <v>44392</v>
+        <v>44551</v>
       </c>
       <c r="M38" t="s">
-        <v>495</v>
+        <v>441</v>
       </c>
       <c r="N38" s="2">
         <v>44551</v>
       </c>
       <c r="O38" t="s">
-        <v>446</v>
-      </c>
-      <c r="P38" s="2">
-        <v>44551</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>497</v>
-      </c>
-      <c r="R38" t="s">
+        <v>491</v>
+      </c>
+      <c r="P38" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>153</v>
       </c>
@@ -4182,29 +4440,32 @@
       <c r="E39">
         <v>30332</v>
       </c>
-      <c r="F39" t="s">
-        <v>457</v>
-      </c>
-      <c r="J39" s="2">
+      <c r="F39" t="b">
+        <v>0</v>
+      </c>
+      <c r="G39" t="s">
+        <v>452</v>
+      </c>
+      <c r="H39" s="2">
         <v>43902</v>
       </c>
-      <c r="K39" s="1" t="s">
-        <v>499</v>
+      <c r="I39" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="J39" t="s">
+        <v>418</v>
       </c>
       <c r="L39" t="s">
-        <v>423</v>
-      </c>
-      <c r="N39" t="s">
-        <v>423</v>
-      </c>
-      <c r="P39" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="R39" t="s">
+        <v>418</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="P39" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>156</v>
       </c>
@@ -4220,38 +4481,41 @@
       <c r="E40">
         <v>95616</v>
       </c>
-      <c r="F40" t="s">
-        <v>457</v>
+      <c r="F40" t="b">
+        <v>0</v>
+      </c>
+      <c r="G40" t="s">
+        <v>452</v>
+      </c>
+      <c r="H40" s="2">
+        <v>43902</v>
+      </c>
+      <c r="I40" t="s">
+        <v>495</v>
       </c>
       <c r="J40" s="2">
-        <v>43902</v>
-      </c>
-      <c r="K40" t="s">
-        <v>501</v>
+        <v>44392</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>433</v>
       </c>
       <c r="L40" s="2">
-        <v>44392</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>438</v>
+        <v>44551</v>
+      </c>
+      <c r="M40" t="s">
+        <v>441</v>
       </c>
       <c r="N40" s="2">
         <v>44551</v>
       </c>
       <c r="O40" t="s">
-        <v>446</v>
-      </c>
-      <c r="P40" s="2">
-        <v>44551</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>500</v>
-      </c>
-      <c r="R40" t="s">
+        <v>494</v>
+      </c>
+      <c r="P40" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>159</v>
       </c>
@@ -4267,29 +4531,32 @@
       <c r="E41">
         <v>78705</v>
       </c>
-      <c r="F41" t="s">
-        <v>457</v>
-      </c>
-      <c r="J41" s="2">
+      <c r="F41" t="b">
+        <v>0</v>
+      </c>
+      <c r="G41" t="s">
+        <v>452</v>
+      </c>
+      <c r="H41" s="2">
         <v>43907</v>
       </c>
-      <c r="K41" t="s">
-        <v>504</v>
+      <c r="I41" t="s">
+        <v>498</v>
+      </c>
+      <c r="J41" t="s">
+        <v>418</v>
       </c>
       <c r="L41" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="N41" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="P41" t="s">
-        <v>423</v>
-      </c>
-      <c r="R41" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>162</v>
       </c>
@@ -4305,35 +4572,38 @@
       <c r="E42">
         <v>23187</v>
       </c>
-      <c r="F42" t="s">
-        <v>457</v>
+      <c r="F42" t="b">
+        <v>0</v>
+      </c>
+      <c r="G42" t="s">
+        <v>452</v>
+      </c>
+      <c r="H42" s="2">
+        <v>43901</v>
+      </c>
+      <c r="I42" t="s">
+        <v>500</v>
       </c>
       <c r="J42" s="2">
-        <v>43901</v>
+        <v>44406</v>
       </c>
       <c r="K42" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="L42" s="2">
-        <v>44406</v>
+        <v>44561</v>
       </c>
       <c r="M42" t="s">
-        <v>505</v>
-      </c>
-      <c r="N42" s="2">
-        <v>44561</v>
-      </c>
-      <c r="O42" t="s">
-        <v>505</v>
+        <v>499</v>
+      </c>
+      <c r="N42" t="s">
+        <v>418</v>
       </c>
       <c r="P42" t="s">
-        <v>423</v>
-      </c>
-      <c r="R42" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>165</v>
       </c>
@@ -4349,32 +4619,35 @@
       <c r="E43">
         <v>2215</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" t="b">
+        <v>0</v>
+      </c>
+      <c r="G43" t="s">
         <v>366</v>
       </c>
+      <c r="H43" s="2">
+        <v>43901</v>
+      </c>
+      <c r="I43" t="s">
+        <v>503</v>
+      </c>
       <c r="J43" s="2">
-        <v>43901</v>
+        <v>44295</v>
       </c>
       <c r="K43" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="L43" s="2">
-        <v>44295</v>
+        <v>44540</v>
       </c>
       <c r="M43" t="s">
-        <v>508</v>
-      </c>
-      <c r="N43" s="2">
-        <v>44540</v>
-      </c>
-      <c r="O43" t="s">
-        <v>507</v>
-      </c>
-      <c r="R43" t="s">
+        <v>501</v>
+      </c>
+      <c r="P43" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>169</v>
       </c>
@@ -4390,35 +4663,38 @@
       <c r="E44">
         <v>2454</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" t="b">
+        <v>0</v>
+      </c>
+      <c r="G44" t="s">
         <v>366</v>
       </c>
+      <c r="H44" s="2">
+        <v>43901</v>
+      </c>
+      <c r="I44" t="s">
+        <v>505</v>
+      </c>
       <c r="J44" s="2">
-        <v>43901</v>
+        <v>44312</v>
       </c>
       <c r="K44" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="L44" s="2">
-        <v>44312</v>
+        <v>44551</v>
       </c>
       <c r="M44" t="s">
-        <v>510</v>
-      </c>
-      <c r="N44" s="2">
-        <v>44551</v>
-      </c>
-      <c r="O44" t="s">
-        <v>512</v>
-      </c>
-      <c r="P44" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="R44" t="s">
+        <v>506</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="P44" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>172</v>
       </c>
@@ -4434,38 +4710,41 @@
       <c r="E45">
         <v>44106</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+      <c r="G45" t="s">
         <v>366</v>
       </c>
+      <c r="H45" s="2">
+        <v>43900</v>
+      </c>
+      <c r="I45" t="s">
+        <v>512</v>
+      </c>
       <c r="J45" s="2">
-        <v>43900</v>
+        <v>44392</v>
       </c>
       <c r="K45" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="L45" s="2">
-        <v>44392</v>
+        <v>44547</v>
       </c>
       <c r="M45" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="N45" s="2">
-        <v>44547</v>
+        <v>44553</v>
       </c>
       <c r="O45" t="s">
-        <v>515</v>
-      </c>
-      <c r="P45" s="2">
-        <v>44553</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>516</v>
-      </c>
-      <c r="R45" t="s">
+        <v>510</v>
+      </c>
+      <c r="P45" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>176</v>
       </c>
@@ -4481,38 +4760,41 @@
       <c r="E46">
         <v>70118</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" t="b">
+        <v>0</v>
+      </c>
+      <c r="G46" t="s">
         <v>366</v>
       </c>
+      <c r="H46" s="2">
+        <v>43901</v>
+      </c>
+      <c r="I46" t="s">
+        <v>515</v>
+      </c>
       <c r="J46" s="2">
-        <v>43901</v>
+        <v>44329</v>
       </c>
       <c r="K46" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
       <c r="L46" s="2">
-        <v>44329</v>
+        <v>44553</v>
       </c>
       <c r="M46" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
       <c r="N46" s="2">
         <v>44553</v>
       </c>
       <c r="O46" t="s">
-        <v>519</v>
-      </c>
-      <c r="P46" s="2">
-        <v>44553</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>519</v>
-      </c>
-      <c r="R46" t="s">
+        <v>513</v>
+      </c>
+      <c r="P46" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>180</v>
       </c>
@@ -4528,29 +4810,32 @@
       <c r="E47">
         <v>53706</v>
       </c>
-      <c r="F47" t="s">
-        <v>457</v>
-      </c>
-      <c r="J47" s="2">
+      <c r="F47" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47" t="s">
+        <v>452</v>
+      </c>
+      <c r="H47" s="2">
         <v>43901</v>
       </c>
-      <c r="K47" t="s">
-        <v>522</v>
+      <c r="I47" t="s">
+        <v>516</v>
+      </c>
+      <c r="J47" t="s">
+        <v>418</v>
       </c>
       <c r="L47" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="N47" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="P47" t="s">
-        <v>423</v>
-      </c>
-      <c r="R47" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>184</v>
       </c>
@@ -4566,35 +4851,38 @@
       <c r="E48">
         <v>61820</v>
       </c>
-      <c r="F48" t="s">
-        <v>457</v>
+      <c r="F48" t="b">
+        <v>0</v>
+      </c>
+      <c r="G48" t="s">
+        <v>452</v>
+      </c>
+      <c r="H48" s="2">
+        <v>43901</v>
+      </c>
+      <c r="I48" t="s">
+        <v>520</v>
       </c>
       <c r="J48" s="2">
-        <v>43901</v>
+        <v>44368</v>
       </c>
       <c r="K48" t="s">
-        <v>526</v>
-      </c>
-      <c r="L48" s="2">
-        <v>44368</v>
-      </c>
-      <c r="M48" t="s">
-        <v>523</v>
-      </c>
-      <c r="N48" t="s">
-        <v>524</v>
-      </c>
-      <c r="P48" s="2">
+        <v>517</v>
+      </c>
+      <c r="L48" t="s">
+        <v>518</v>
+      </c>
+      <c r="N48" s="2">
         <v>44550</v>
       </c>
-      <c r="Q48" s="1" t="s">
-        <v>525</v>
-      </c>
-      <c r="R48" t="s">
+      <c r="O48" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="P48" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>188</v>
       </c>
@@ -4610,29 +4898,32 @@
       <c r="E49">
         <v>30602</v>
       </c>
-      <c r="F49" t="s">
-        <v>457</v>
-      </c>
-      <c r="J49" s="2">
+      <c r="F49" t="b">
+        <v>0</v>
+      </c>
+      <c r="G49" t="s">
+        <v>452</v>
+      </c>
+      <c r="H49" s="2">
         <v>43902</v>
       </c>
-      <c r="K49" t="s">
-        <v>527</v>
+      <c r="I49" t="s">
+        <v>521</v>
+      </c>
+      <c r="J49" t="s">
+        <v>418</v>
       </c>
       <c r="L49" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="N49" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="P49" t="s">
-        <v>423</v>
-      </c>
-      <c r="R49" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>192</v>
       </c>
@@ -4648,35 +4939,38 @@
       <c r="E50">
         <v>18015</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" t="b">
+        <v>0</v>
+      </c>
+      <c r="G50" t="s">
         <v>366</v>
       </c>
+      <c r="H50" s="2">
+        <v>43901</v>
+      </c>
+      <c r="I50" t="s">
+        <v>524</v>
+      </c>
       <c r="J50" s="2">
-        <v>43901</v>
+        <v>44307</v>
       </c>
       <c r="K50" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="L50" s="2">
-        <v>44307</v>
+        <v>44552</v>
       </c>
       <c r="M50" t="s">
-        <v>529</v>
-      </c>
-      <c r="N50" s="2">
-        <v>44552</v>
-      </c>
-      <c r="O50" t="s">
-        <v>528</v>
+        <v>522</v>
+      </c>
+      <c r="N50" t="s">
+        <v>418</v>
       </c>
       <c r="P50" t="s">
-        <v>423</v>
-      </c>
-      <c r="R50" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>196</v>
       </c>
@@ -4692,35 +4986,38 @@
       <c r="E51">
         <v>2115</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" t="b">
+        <v>0</v>
+      </c>
+      <c r="G51" t="s">
         <v>366</v>
       </c>
+      <c r="H51" s="2">
+        <v>43901</v>
+      </c>
+      <c r="I51" t="s">
+        <v>527</v>
+      </c>
       <c r="J51" s="2">
-        <v>43901</v>
+        <v>44292</v>
       </c>
       <c r="K51" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="L51" s="2">
-        <v>44292</v>
+        <v>44539</v>
       </c>
       <c r="M51" t="s">
-        <v>532</v>
-      </c>
-      <c r="N51" s="2">
-        <v>44539</v>
-      </c>
-      <c r="O51" t="s">
-        <v>531</v>
+        <v>525</v>
+      </c>
+      <c r="N51" t="s">
+        <v>418</v>
       </c>
       <c r="P51" t="s">
-        <v>423</v>
-      </c>
-      <c r="R51" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>198</v>
       </c>
@@ -4736,32 +5033,35 @@
       <c r="E52">
         <v>43210</v>
       </c>
-      <c r="F52" t="s">
-        <v>457</v>
+      <c r="F52" t="b">
+        <v>0</v>
+      </c>
+      <c r="G52" t="s">
+        <v>452</v>
+      </c>
+      <c r="H52" s="2">
+        <v>43899</v>
+      </c>
+      <c r="I52" t="s">
+        <v>529</v>
       </c>
       <c r="J52" s="2">
-        <v>43899</v>
+        <v>44432</v>
       </c>
       <c r="K52" t="s">
-        <v>535</v>
-      </c>
-      <c r="L52" s="2">
-        <v>44432</v>
-      </c>
-      <c r="M52" t="s">
-        <v>534</v>
+        <v>528</v>
+      </c>
+      <c r="L52" t="s">
+        <v>418</v>
       </c>
       <c r="N52" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="P52" t="s">
-        <v>423</v>
-      </c>
-      <c r="R52" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>201</v>
       </c>
@@ -4777,14 +5077,17 @@
       <c r="E53">
         <v>90263</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G53" t="s">
         <v>366</v>
       </c>
-      <c r="R53" t="s">
+      <c r="P53" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>204</v>
       </c>
@@ -4800,14 +5103,17 @@
       <c r="E54">
         <v>47907</v>
       </c>
-      <c r="F54" t="s">
-        <v>457</v>
-      </c>
-      <c r="R54" t="s">
+      <c r="F54" t="b">
+        <v>0</v>
+      </c>
+      <c r="G54" t="s">
+        <v>452</v>
+      </c>
+      <c r="P54" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>207</v>
       </c>
@@ -4823,14 +5129,17 @@
       <c r="E55">
         <v>19085</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" t="b">
+        <v>0</v>
+      </c>
+      <c r="G55" t="s">
         <v>366</v>
       </c>
-      <c r="R55" t="s">
+      <c r="P55" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>210</v>
       </c>
@@ -4846,14 +5155,14 @@
       <c r="E56">
         <v>32306</v>
       </c>
-      <c r="F56" t="s">
-        <v>366</v>
-      </c>
-      <c r="R56" t="s">
+      <c r="F56" t="b">
+        <v>0</v>
+      </c>
+      <c r="P56" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>214</v>
       </c>
@@ -4869,14 +5178,14 @@
       <c r="E57">
         <v>12180</v>
       </c>
-      <c r="F57" t="s">
-        <v>366</v>
-      </c>
-      <c r="R57" t="s">
+      <c r="F57" t="b">
+        <v>0</v>
+      </c>
+      <c r="P57" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>217</v>
       </c>
@@ -4892,14 +5201,14 @@
       <c r="E58">
         <v>95053</v>
       </c>
-      <c r="F58" t="s">
-        <v>366</v>
-      </c>
-      <c r="R58" t="s">
+      <c r="F58" t="b">
+        <v>0</v>
+      </c>
+      <c r="P58" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>220</v>
       </c>
@@ -4915,14 +5224,14 @@
       <c r="E59">
         <v>33124</v>
       </c>
-      <c r="F59" t="s">
-        <v>366</v>
-      </c>
-      <c r="R59" t="s">
+      <c r="F59" t="b">
+        <v>0</v>
+      </c>
+      <c r="P59" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>223</v>
       </c>
@@ -4938,14 +5247,14 @@
       <c r="E60">
         <v>13244</v>
       </c>
-      <c r="F60" t="s">
-        <v>366</v>
-      </c>
-      <c r="R60" t="s">
+      <c r="F60" t="b">
+        <v>0</v>
+      </c>
+      <c r="P60" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>227</v>
       </c>
@@ -4961,14 +5270,14 @@
       <c r="E61">
         <v>20742</v>
       </c>
-      <c r="F61" t="s">
-        <v>366</v>
-      </c>
-      <c r="R61" t="s">
+      <c r="F61" t="b">
+        <v>0</v>
+      </c>
+      <c r="P61" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>230</v>
       </c>
@@ -4984,14 +5293,14 @@
       <c r="E62">
         <v>15260</v>
       </c>
-      <c r="F62" t="s">
-        <v>366</v>
-      </c>
-      <c r="R62" t="s">
+      <c r="F62" t="b">
+        <v>0</v>
+      </c>
+      <c r="P62" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>232</v>
       </c>
@@ -5007,14 +5316,14 @@
       <c r="E63">
         <v>98195</v>
       </c>
-      <c r="F63" t="s">
-        <v>366</v>
-      </c>
-      <c r="R63" t="s">
+      <c r="F63" t="b">
+        <v>0</v>
+      </c>
+      <c r="P63" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>236</v>
       </c>
@@ -5030,14 +5339,14 @@
       <c r="E64">
         <v>20052</v>
       </c>
-      <c r="F64" t="s">
-        <v>366</v>
-      </c>
-      <c r="R64" t="s">
+      <c r="F64" t="b">
+        <v>0</v>
+      </c>
+      <c r="P64" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>239</v>
       </c>
@@ -5053,14 +5362,14 @@
       <c r="E65">
         <v>16802</v>
       </c>
-      <c r="F65" t="s">
-        <v>366</v>
-      </c>
-      <c r="R65" t="s">
+      <c r="F65" t="b">
+        <v>0</v>
+      </c>
+      <c r="P65" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>242</v>
       </c>
@@ -5076,14 +5385,14 @@
       <c r="E66">
         <v>8854</v>
       </c>
-      <c r="F66" t="s">
-        <v>366</v>
-      </c>
-      <c r="R66" t="s">
+      <c r="F66" t="b">
+        <v>0</v>
+      </c>
+      <c r="P66" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>245</v>
       </c>
@@ -5099,14 +5408,14 @@
       <c r="E67">
         <v>6269</v>
       </c>
-      <c r="F67" t="s">
-        <v>366</v>
-      </c>
-      <c r="R67" t="s">
+      <c r="F67" t="b">
+        <v>0</v>
+      </c>
+      <c r="P67" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>248</v>
       </c>
@@ -5122,14 +5431,14 @@
       <c r="E68">
         <v>1609</v>
       </c>
-      <c r="F68" t="s">
-        <v>366</v>
-      </c>
-      <c r="R68" t="s">
+      <c r="F68" t="b">
+        <v>0</v>
+      </c>
+      <c r="P68" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>251</v>
       </c>
@@ -5145,14 +5454,14 @@
       <c r="E69">
         <v>10023</v>
       </c>
-      <c r="F69" t="s">
-        <v>366</v>
-      </c>
-      <c r="R69" t="s">
+      <c r="F69" t="b">
+        <v>0</v>
+      </c>
+      <c r="P69" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>254</v>
       </c>
@@ -5168,14 +5477,14 @@
       <c r="E70">
         <v>47405</v>
       </c>
-      <c r="F70" t="s">
-        <v>366</v>
-      </c>
-      <c r="R70" t="s">
+      <c r="F70" t="b">
+        <v>0</v>
+      </c>
+      <c r="P70" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>257</v>
       </c>
@@ -5191,14 +5500,14 @@
       <c r="E71">
         <v>75275</v>
       </c>
-      <c r="F71" t="s">
-        <v>366</v>
-      </c>
-      <c r="R71" t="s">
+      <c r="F71" t="b">
+        <v>0</v>
+      </c>
+      <c r="P71" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>260</v>
       </c>
@@ -5214,14 +5523,14 @@
       <c r="E72">
         <v>77843</v>
       </c>
-      <c r="F72" t="s">
-        <v>366</v>
-      </c>
-      <c r="R72" t="s">
+      <c r="F72" t="b">
+        <v>0</v>
+      </c>
+      <c r="P72" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>263</v>
       </c>
@@ -5237,14 +5546,14 @@
       <c r="E73">
         <v>1003</v>
       </c>
-      <c r="F73" t="s">
-        <v>366</v>
-      </c>
-      <c r="R73" t="s">
+      <c r="F73" t="b">
+        <v>0</v>
+      </c>
+      <c r="P73" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>266</v>
       </c>
@@ -5260,14 +5569,14 @@
       <c r="E74">
         <v>55455</v>
       </c>
-      <c r="F74" t="s">
-        <v>366</v>
-      </c>
-      <c r="R74" t="s">
+      <c r="F74" t="b">
+        <v>0</v>
+      </c>
+      <c r="P74" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>270</v>
       </c>
@@ -5283,14 +5592,14 @@
       <c r="E75">
         <v>10033</v>
       </c>
-      <c r="F75" t="s">
-        <v>366</v>
-      </c>
-      <c r="R75" t="s">
+      <c r="F75" t="b">
+        <v>0</v>
+      </c>
+      <c r="P75" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>272</v>
       </c>
@@ -5306,14 +5615,14 @@
       <c r="E76">
         <v>76798</v>
       </c>
-      <c r="F76" t="s">
-        <v>366</v>
-      </c>
-      <c r="R76" t="s">
+      <c r="F76" t="b">
+        <v>0</v>
+      </c>
+      <c r="P76" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>276</v>
       </c>
@@ -5329,14 +5638,14 @@
       <c r="E77">
         <v>29634</v>
       </c>
-      <c r="F77" t="s">
-        <v>366</v>
-      </c>
-      <c r="R77" t="s">
+      <c r="F77" t="b">
+        <v>0</v>
+      </c>
+      <c r="P77" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>280</v>
       </c>
@@ -5352,14 +5661,14 @@
       <c r="E78">
         <v>90045</v>
       </c>
-      <c r="F78" t="s">
-        <v>366</v>
-      </c>
-      <c r="R78" t="s">
+      <c r="F78" t="b">
+        <v>0</v>
+      </c>
+      <c r="P78" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>282</v>
       </c>
@@ -5375,14 +5684,14 @@
       <c r="E79">
         <v>24061</v>
       </c>
-      <c r="F79" t="s">
-        <v>366</v>
-      </c>
-      <c r="R79" t="s">
+      <c r="F79" t="b">
+        <v>0</v>
+      </c>
+      <c r="P79" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>285</v>
       </c>
@@ -5398,14 +5707,14 @@
       <c r="E80">
         <v>20016</v>
       </c>
-      <c r="F80" t="s">
-        <v>366</v>
-      </c>
-      <c r="R80" t="s">
+      <c r="F80" t="b">
+        <v>0</v>
+      </c>
+      <c r="P80" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>288</v>
       </c>
@@ -5421,14 +5730,14 @@
       <c r="E81">
         <v>84602</v>
       </c>
-      <c r="F81" t="s">
-        <v>366</v>
-      </c>
-      <c r="R81" t="s">
+      <c r="F81" t="b">
+        <v>0</v>
+      </c>
+      <c r="P81" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>292</v>
       </c>
@@ -5444,14 +5753,14 @@
       <c r="E82">
         <v>99258</v>
       </c>
-      <c r="F82" t="s">
-        <v>366</v>
-      </c>
-      <c r="R82" t="s">
+      <c r="F82" t="b">
+        <v>0</v>
+      </c>
+      <c r="P82" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>295</v>
       </c>
@@ -5467,14 +5776,14 @@
       <c r="E83">
         <v>27695</v>
       </c>
-      <c r="F83" t="s">
-        <v>366</v>
-      </c>
-      <c r="R83" t="s">
+      <c r="F83" t="b">
+        <v>0</v>
+      </c>
+      <c r="P83" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>298</v>
       </c>
@@ -5490,14 +5799,14 @@
       <c r="E84">
         <v>13902</v>
       </c>
-      <c r="F84" t="s">
-        <v>366</v>
-      </c>
-      <c r="R84" t="s">
+      <c r="F84" t="b">
+        <v>0</v>
+      </c>
+      <c r="P84" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>302</v>
       </c>
@@ -5513,14 +5822,14 @@
       <c r="E85">
         <v>80401</v>
       </c>
-      <c r="F85" t="s">
-        <v>366</v>
-      </c>
-      <c r="R85" t="s">
+      <c r="F85" t="b">
+        <v>0</v>
+      </c>
+      <c r="P85" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>306</v>
       </c>
@@ -5536,14 +5845,14 @@
       <c r="E86">
         <v>27244</v>
       </c>
-      <c r="F86" t="s">
-        <v>366</v>
-      </c>
-      <c r="R86" t="s">
+      <c r="F86" t="b">
+        <v>0</v>
+      </c>
+      <c r="P86" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>309</v>
       </c>
@@ -5559,14 +5868,14 @@
       <c r="E87">
         <v>20059</v>
       </c>
-      <c r="F87" t="s">
-        <v>366</v>
-      </c>
-      <c r="R87" t="s">
+      <c r="F87" t="b">
+        <v>0</v>
+      </c>
+      <c r="P87" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>311</v>
       </c>
@@ -5582,14 +5891,14 @@
       <c r="E88">
         <v>53201</v>
       </c>
-      <c r="F88" t="s">
-        <v>366</v>
-      </c>
-      <c r="R88" t="s">
+      <c r="F88" t="b">
+        <v>0</v>
+      </c>
+      <c r="P88" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>314</v>
       </c>
@@ -5605,14 +5914,14 @@
       <c r="E89">
         <v>48824</v>
       </c>
-      <c r="F89" t="s">
-        <v>366</v>
-      </c>
-      <c r="R89" t="s">
+      <c r="F89" t="b">
+        <v>0</v>
+      </c>
+      <c r="P89" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>317</v>
       </c>
@@ -5628,14 +5937,14 @@
       <c r="E90">
         <v>7030</v>
       </c>
-      <c r="F90" t="s">
-        <v>366</v>
-      </c>
-      <c r="R90" t="s">
+      <c r="F90" t="b">
+        <v>0</v>
+      </c>
+      <c r="P90" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>320</v>
       </c>
@@ -5651,14 +5960,14 @@
       <c r="E91">
         <v>76129</v>
       </c>
-      <c r="F91" t="s">
-        <v>366</v>
-      </c>
-      <c r="R91" t="s">
+      <c r="F91" t="b">
+        <v>0</v>
+      </c>
+      <c r="P91" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>323</v>
       </c>
@@ -5674,14 +5983,14 @@
       <c r="E92">
         <v>92521</v>
       </c>
-      <c r="F92" t="s">
-        <v>366</v>
-      </c>
-      <c r="R92" t="s">
+      <c r="F92" t="b">
+        <v>0</v>
+      </c>
+      <c r="P92" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>326</v>
       </c>
@@ -5697,14 +6006,14 @@
       <c r="E93">
         <v>52242</v>
       </c>
-      <c r="F93" t="s">
-        <v>366</v>
-      </c>
-      <c r="R93" t="s">
+      <c r="F93" t="b">
+        <v>0</v>
+      </c>
+      <c r="P93" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>330</v>
       </c>
@@ -5720,14 +6029,14 @@
       <c r="E94">
         <v>11794</v>
       </c>
-      <c r="F94" t="s">
-        <v>366</v>
-      </c>
-      <c r="R94" t="s">
+      <c r="F94" t="b">
+        <v>0</v>
+      </c>
+      <c r="P94" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>334</v>
       </c>
@@ -5743,14 +6052,14 @@
       <c r="E95">
         <v>14214</v>
       </c>
-      <c r="F95" t="s">
-        <v>366</v>
-      </c>
-      <c r="R95" t="s">
+      <c r="F95" t="b">
+        <v>0</v>
+      </c>
+      <c r="P95" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>337</v>
       </c>
@@ -5766,14 +6075,14 @@
       <c r="E96">
         <v>95343</v>
       </c>
-      <c r="F96" t="s">
-        <v>366</v>
-      </c>
-      <c r="R96" t="s">
+      <c r="F96" t="b">
+        <v>0</v>
+      </c>
+      <c r="P96" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>340</v>
       </c>
@@ -5789,14 +6098,14 @@
       <c r="E97">
         <v>19716</v>
       </c>
-      <c r="F97" t="s">
-        <v>366</v>
-      </c>
-      <c r="R97" t="s">
+      <c r="F97" t="b">
+        <v>0</v>
+      </c>
+      <c r="P97" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>344</v>
       </c>
@@ -5812,14 +6121,14 @@
       <c r="E98">
         <v>80208</v>
       </c>
-      <c r="F98" t="s">
-        <v>366</v>
-      </c>
-      <c r="R98" t="s">
+      <c r="F98" t="b">
+        <v>0</v>
+      </c>
+      <c r="P98" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>347</v>
       </c>
@@ -5835,14 +6144,14 @@
       <c r="E99">
         <v>92110</v>
       </c>
-      <c r="F99" t="s">
-        <v>366</v>
-      </c>
-      <c r="R99" t="s">
+      <c r="F99" t="b">
+        <v>0</v>
+      </c>
+      <c r="P99" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>350</v>
       </c>
@@ -5858,14 +6167,14 @@
       <c r="E100">
         <v>36849</v>
       </c>
-      <c r="F100" t="s">
-        <v>366</v>
-      </c>
-      <c r="R100" t="s">
+      <c r="F100" t="b">
+        <v>0</v>
+      </c>
+      <c r="P100" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>355</v>
       </c>
@@ -5881,14 +6190,14 @@
       <c r="E101">
         <v>80309</v>
       </c>
-      <c r="F101" t="s">
-        <v>366</v>
-      </c>
-      <c r="R101" t="s">
+      <c r="F101" t="b">
+        <v>0</v>
+      </c>
+      <c r="P101" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>358</v>
       </c>
@@ -5904,14 +6213,14 @@
       <c r="E102">
         <v>97403</v>
       </c>
-      <c r="F102" t="s">
-        <v>366</v>
-      </c>
-      <c r="R102" t="s">
+      <c r="F102" t="b">
+        <v>0</v>
+      </c>
+      <c r="P102" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>362</v>
       </c>
@@ -5927,35 +6236,35 @@
       <c r="E103">
         <v>84112</v>
       </c>
-      <c r="F103" t="s">
-        <v>366</v>
-      </c>
-      <c r="R103" t="s">
+      <c r="F103" t="b">
+        <v>0</v>
+      </c>
+      <c r="P103" t="s">
         <v>364</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="M2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="O2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="K5" r:id="rId4" xr:uid="{63B74F0C-B244-4A83-ACCA-FA3F68184AC5}"/>
-    <hyperlink ref="O6" r:id="rId5" xr:uid="{B0F35A6A-7F82-4802-B279-01342AA58C8C}"/>
-    <hyperlink ref="O7" r:id="rId6" xr:uid="{F2138E74-A2AC-4426-A25E-63DC99F15DAC}"/>
-    <hyperlink ref="K3" r:id="rId7" xr:uid="{BE01ACE6-FB34-4756-97EA-9581BB15503C}"/>
-    <hyperlink ref="K4" r:id="rId8" xr:uid="{4E3DC3E6-7BC6-478C-B6D8-CBBA262F2910}"/>
-    <hyperlink ref="K6" r:id="rId9" xr:uid="{E09C8912-8079-4FF4-9849-391BA2BAFD0A}"/>
-    <hyperlink ref="K8" r:id="rId10" xr:uid="{17325C6C-78D9-4ECA-932A-FCE4742B6ACB}"/>
-    <hyperlink ref="M8" r:id="rId11" xr:uid="{4AF1C7F1-ED00-411A-BE4C-7267BA178689}"/>
-    <hyperlink ref="M17" r:id="rId12" xr:uid="{3521C5C1-BC8F-4E4B-96DF-8AB4791CE007}"/>
-    <hyperlink ref="K19" r:id="rId13" xr:uid="{34797C79-CF3E-4ED0-8540-829F7FB131FE}"/>
-    <hyperlink ref="K21" r:id="rId14" xr:uid="{71222E2C-FD57-461E-A309-BA2702D58EFB}"/>
-    <hyperlink ref="O23" r:id="rId15" xr:uid="{8BDEC90D-B3D3-440F-9429-03D3BB81F16E}"/>
-    <hyperlink ref="K37" r:id="rId16" xr:uid="{0046736D-A681-4613-AE08-A73A7766DD85}"/>
-    <hyperlink ref="K39" r:id="rId17" xr:uid="{FE66A646-56F4-4AAB-A671-B27FB1D2C36C}"/>
-    <hyperlink ref="M23" r:id="rId18" xr:uid="{964B5D27-CC24-4B35-9697-424685535672}"/>
-    <hyperlink ref="M40" r:id="rId19" xr:uid="{34EC3477-0693-44EE-AC46-2D6F8B875152}"/>
-    <hyperlink ref="Q48" r:id="rId20" xr:uid="{0C817430-0A62-4C61-8AF2-3C031261F73D}"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="M2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="I5" r:id="rId4" xr:uid="{63B74F0C-B244-4A83-ACCA-FA3F68184AC5}"/>
+    <hyperlink ref="M6" r:id="rId5" xr:uid="{B0F35A6A-7F82-4802-B279-01342AA58C8C}"/>
+    <hyperlink ref="M7" r:id="rId6" xr:uid="{F2138E74-A2AC-4426-A25E-63DC99F15DAC}"/>
+    <hyperlink ref="I3" r:id="rId7" xr:uid="{BE01ACE6-FB34-4756-97EA-9581BB15503C}"/>
+    <hyperlink ref="I4" r:id="rId8" xr:uid="{4E3DC3E6-7BC6-478C-B6D8-CBBA262F2910}"/>
+    <hyperlink ref="I6" r:id="rId9" xr:uid="{E09C8912-8079-4FF4-9849-391BA2BAFD0A}"/>
+    <hyperlink ref="I8" r:id="rId10" xr:uid="{17325C6C-78D9-4ECA-932A-FCE4742B6ACB}"/>
+    <hyperlink ref="K8" r:id="rId11" xr:uid="{4AF1C7F1-ED00-411A-BE4C-7267BA178689}"/>
+    <hyperlink ref="K17" r:id="rId12" xr:uid="{3521C5C1-BC8F-4E4B-96DF-8AB4791CE007}"/>
+    <hyperlink ref="I19" r:id="rId13" xr:uid="{34797C79-CF3E-4ED0-8540-829F7FB131FE}"/>
+    <hyperlink ref="I21" r:id="rId14" xr:uid="{71222E2C-FD57-461E-A309-BA2702D58EFB}"/>
+    <hyperlink ref="M23" r:id="rId15" xr:uid="{8BDEC90D-B3D3-440F-9429-03D3BB81F16E}"/>
+    <hyperlink ref="I37" r:id="rId16" xr:uid="{0046736D-A681-4613-AE08-A73A7766DD85}"/>
+    <hyperlink ref="I39" r:id="rId17" xr:uid="{FE66A646-56F4-4AAB-A671-B27FB1D2C36C}"/>
+    <hyperlink ref="K23" r:id="rId18" xr:uid="{964B5D27-CC24-4B35-9697-424685535672}"/>
+    <hyperlink ref="K40" r:id="rId19" xr:uid="{34EC3477-0693-44EE-AC46-2D6F8B875152}"/>
+    <hyperlink ref="O48" r:id="rId20" xr:uid="{0C817430-0A62-4C61-8AF2-3C031261F73D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5983,57 +6292,57 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
     </row>
   </sheetData>

</xml_diff>